<commit_message>
Ajout des test temporels pour la méthode exacte
</commit_message>
<xml_diff>
--- a/3TP/projetRO/Résultats expérimentaux.xlsx
+++ b/3TP/projetRO/Résultats expérimentaux.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mehdilatif/Desktop/ÉTUDES/FAC/S6/RO/TP/3TP/projetRO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{1C487A01-6BD5-A34E-8F81-2EA0F86DDC9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{08D487B0-D22B-AF4E-8E22-6B4FC2D6DD2F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12400" yWindow="0" windowWidth="16120" windowHeight="17560" xr2:uid="{547F177B-E832-2149-833C-BBBB1F24BC1B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{547F177B-E832-2149-833C-BBBB1F24BC1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Exacte" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Plat 10</t>
   </si>
@@ -115,19 +115,127 @@
   </si>
   <si>
     <t>Relief 150</t>
+  </si>
+  <si>
+    <t>Nb Iter</t>
+  </si>
+  <si>
+    <t>Nb Ctr ajoutée</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Tps + CPU</t>
+  </si>
+  <si>
+    <t>0.137014 seconds (5.89 k allocations: 393.406 KiB)</t>
+  </si>
+  <si>
+    <t>0.165501 seconds (26.36 k allocations: 2.154 MiB)</t>
+  </si>
+  <si>
+    <t>0.206548 seconds (57.40 k allocations: 5.059 MiB)</t>
+  </si>
+  <si>
+    <t>1.062222 seconds (123.52 k allocations: 11.635 MiB)</t>
+  </si>
+  <si>
+    <t>3.375432 seconds (311.61 k allocations: 31.073 MiB, 0.18% gc time)</t>
+  </si>
+  <si>
+    <t>0.492398 seconds (195.61 k allocations: 19.725 MiB, 1.01% gc time)</t>
+  </si>
+  <si>
+    <t>17.763255 seconds (667.01 k allocations: 72.797 MiB, 0.10% gc time)</t>
+  </si>
+  <si>
+    <t>6.156659 seconds (685.97 k allocations: 73.051 MiB, 0.29% gc time)</t>
+  </si>
+  <si>
+    <t>7.125538 seconds (911.33 k allocations: 96.495 MiB, 0.28% gc time)</t>
+  </si>
+  <si>
+    <t>41.788991 seconds (1.41 M allocations: 157.975 MiB, 0.38% gc time)</t>
+  </si>
+  <si>
+    <t>35.971777 seconds (2.14 M allocations: 236.806 MiB, 0.13% gc time)</t>
+  </si>
+  <si>
+    <t>105.200705 seconds (3.88 M allocations: 445.682 MiB, 0.08% gc time)</t>
+  </si>
+  <si>
+    <t>12.828082 seconds (1.42 M allocations: 155.523 MiB, 0.27% gc time)</t>
+  </si>
+  <si>
+    <t>45.006563 seconds (2.75 M allocations: 323.459 MiB, 0.14% gc time)</t>
+  </si>
+  <si>
+    <t>74.752989 seconds (3.30 M allocations: 383.730 MiB, 0.25% gc time)</t>
+  </si>
+  <si>
+    <t>  0.130585 seconds (5.89 k allocations: 394.094 KiB)</t>
+  </si>
+  <si>
+    <t>  0.145352 seconds (13.47 k allocations: 937.688 KiB)</t>
+  </si>
+  <si>
+    <t>  0.131483 seconds (6.80 k allocations: 856.938 KiB)</t>
+  </si>
+  <si>
+    <t>  0.155768 seconds (49.13 k allocations: 3.593 MiB)</t>
+  </si>
+  <si>
+    <t>  0.480462 seconds (110.15 k allocations: 9.687 MiB, 1.22% gc time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.478024 seconds (154.46 k allocations: 13.213 MiB, 1.35% gc time)</t>
+  </si>
+  <si>
+    <t>  0.384103 seconds (175.00 k allocations: 14.856 MiB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.156912 seconds (296.54 k allocations: 26.947 MiB, 0.99% gc time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.976702 seconds (302.92 k allocations: 25.066 MiB, 0.66% gc time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3.671390 seconds (521.89 k allocations: 50.510 MiB, 0.50% gc time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1.016204 seconds (399.29 k allocations: 31.878 MiB, 0.65% gc time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2.732261 seconds (655.98 k allocations: 58.963 MiB, 0.89% gc time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0.819629 seconds (487.95 k allocations: 38.457 MiB, 1.75% gc time)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  9.981334 seconds (1.30 M allocations: 134.869 MiB, 1.38% gc time)</t>
+  </si>
+  <si>
+    <t>  3.296910 seconds (1.02 M allocations: 94.883 MiB, 1.07% gc time)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -150,8 +258,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,165 +575,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1E17BB-6991-4349-B8E8-0823C82541ED}">
-  <dimension ref="A2:A32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:5">
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="C2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="C4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="C7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="C15" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="C19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="C20" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="C23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
+      <c r="C24" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
+      <c r="C26" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
+      <c r="C28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
+      <c r="C29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
+      <c r="C30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
+      <c r="C31" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>